<commit_message>
add visualization and some tools
</commit_message>
<xml_diff>
--- a/dataset/simple/LP_spreadsheet.xlsx
+++ b/dataset/simple/LP_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62ca1cae374228d5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yueqian/Documents/VRPTW-gurobipy/dataset/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2366" documentId="13_ncr:1_{187A7F80-1BA6-4602-A62A-37E8AEA0C148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21990453-9204-45A8-AA46-1DCF50F7AC9F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599ABAE8-115F-4042-9009-A469038A1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{1CD4BA9A-CE17-4CF2-91AB-C507240267C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1CD4BA9A-CE17-4CF2-91AB-C507240267C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,12 +73,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -146,9 +143,6 @@
   </si>
   <si>
     <t>demand</t>
-  </si>
-  <si>
-    <t>cargo use</t>
   </si>
   <si>
     <t>act. dist.</t>
@@ -221,6 +215,9 @@
   </si>
   <si>
     <t>data and parameter</t>
+  </si>
+  <si>
+    <t>cargo</t>
   </si>
 </sst>
 </file>
@@ -692,18 +689,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,14 +718,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -733,18 +742,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
@@ -1003,7 +1000,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="543873551"/>
@@ -1065,7 +1062,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="543858575"/>
@@ -1113,7 +1110,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2020,19 +2017,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1127FEC4-A398-4C78-A3AF-164ECE0A8BD6}">
   <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42.1796875" customWidth="1"/>
-    <col min="27" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.1640625" customWidth="1"/>
+    <col min="27" max="27" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -2069,16 +2066,16 @@
       <c r="P2" s="15"/>
       <c r="Q2" s="18"/>
       <c r="Z2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA2" s="38">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="29">
         <f>$K$7*SUM(M41:Q45,M48:Q52)</f>
         <v>66.502815398728842</v>
       </c>
       <c r="AB2" s="15"/>
       <c r="AC2" s="18"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="1">
         <v>0</v>
@@ -2110,18 +2107,18 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="20"/>
-      <c r="Z3" s="46"/>
+      <c r="Z3" s="34"/>
       <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
-      <c r="AC3" s="47"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AC3" s="35"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="4">
         <v>1</v>
@@ -2153,27 +2150,27 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="20"/>
       <c r="Z4" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA4" s="8">
         <f>SUM(C42:G42,C49:G49)</f>
         <v>1</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC4" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="1">
         <v>2</v>
@@ -2215,13 +2212,13 @@
         <v>1</v>
       </c>
       <c r="AB5" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC5" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="4">
         <v>3</v>
@@ -2257,19 +2254,19 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="20"/>
-      <c r="Z6" s="46"/>
+      <c r="Z6" s="34"/>
       <c r="AA6" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC6" s="47">
+        <v>28</v>
+      </c>
+      <c r="AC6" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="1">
         <v>4</v>
@@ -2294,7 +2291,7 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" s="8">
         <v>1</v>
@@ -2306,20 +2303,20 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="20"/>
       <c r="Z7" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA7" s="8">
         <f>SUM(C41:G41)</f>
         <v>1</v>
       </c>
       <c r="AB7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC7" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2337,19 +2334,19 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="20"/>
-      <c r="Z8" s="46"/>
+      <c r="Z8" s="34"/>
       <c r="AA8" s="10">
         <f>SUM(C48:G48)</f>
         <v>1</v>
       </c>
       <c r="AB8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC8" s="47">
+        <v>28</v>
+      </c>
+      <c r="AC8" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -2385,20 +2382,20 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="20"/>
       <c r="Z9" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA9" s="8">
         <f>SUM(G41:G45)</f>
         <v>1</v>
       </c>
       <c r="AB9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC9" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="8" t="s">
         <v>9</v>
@@ -2433,19 +2430,19 @@
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="20"/>
-      <c r="Z10" s="46"/>
+      <c r="Z10" s="34"/>
       <c r="AA10" s="10">
         <f>SUM(G48:G52)</f>
         <v>1</v>
       </c>
       <c r="AB10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC10" s="47">
+        <v>28</v>
+      </c>
+      <c r="AC10" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2464,37 +2461,37 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="20"/>
       <c r="Z11" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA11" s="8">
         <f>SUM(D41:D45)-SUM(C42:G42)</f>
         <v>0</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC11" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="39">
-        <v>0</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="C12" s="30">
+        <v>0</v>
+      </c>
+      <c r="D12" s="30">
         <v>1</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="30">
         <v>2</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="30">
         <v>3</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="30">
         <v>4</v>
       </c>
       <c r="H12" s="8"/>
@@ -2513,13 +2510,13 @@
         <v>0</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC12" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="21">
         <v>0</v>
@@ -2560,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="AB13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC13" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="8">
         <v>1</v>
@@ -2607,13 +2604,13 @@
         <v>0</v>
       </c>
       <c r="AB14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC14" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="21">
         <v>2</v>
@@ -2654,13 +2651,13 @@
         <v>0</v>
       </c>
       <c r="AB15" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC15" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="8">
         <v>3</v>
@@ -2695,19 +2692,19 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="20"/>
-      <c r="Z16" s="46"/>
+      <c r="Z16" s="34"/>
       <c r="AA16" s="10">
         <f>SUM(F48:F52)-SUM(C51:G51)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC16" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="AC16" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="21">
         <v>4</v>
@@ -2743,21 +2740,21 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="20"/>
       <c r="Z17" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA17" s="8">
         <f>SUM(J41:J45)</f>
         <v>20</v>
       </c>
       <c r="AB17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC17" s="20">
         <f>$K$6</f>
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2775,37 +2772,37 @@
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="20"/>
-      <c r="Z18" s="46"/>
+      <c r="Z18" s="34"/>
       <c r="AA18" s="10">
         <f>SUM(J48:J52)</f>
         <v>10</v>
       </c>
       <c r="AB18" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC18" s="47">
+        <v>34</v>
+      </c>
+      <c r="AC18" s="35">
         <f>$K$6</f>
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="39">
-        <v>0</v>
-      </c>
-      <c r="D19" s="39">
+      <c r="C19" s="30">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30">
         <v>1</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="30">
         <v>2</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="30">
         <v>3</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="30">
         <v>4</v>
       </c>
       <c r="H19" s="8"/>
@@ -2819,9 +2816,9 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="20"/>
       <c r="Z19" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA19" s="48">
+        <v>35</v>
+      </c>
+      <c r="AA19" s="36">
         <v>0</v>
       </c>
       <c r="AB19" s="8">
@@ -2833,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="21">
         <v>0</v>
@@ -2869,7 +2866,7 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="20"/>
       <c r="Z20" s="19"/>
-      <c r="AA20" s="37">
+      <c r="AA20" s="28">
         <v>10</v>
       </c>
       <c r="AB20" s="8">
@@ -2881,7 +2878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="8">
         <v>1</v>
@@ -2917,7 +2914,7 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="20"/>
       <c r="Z21" s="19"/>
-      <c r="AA21" s="37">
+      <c r="AA21" s="28">
         <v>20</v>
       </c>
       <c r="AB21" s="8">
@@ -2929,7 +2926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="21">
         <v>2</v>
@@ -2965,7 +2962,7 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="20"/>
       <c r="Z22" s="19"/>
-      <c r="AA22" s="37">
+      <c r="AA22" s="28">
         <v>52.36067977501078</v>
       </c>
       <c r="AB22" s="8">
@@ -2977,7 +2974,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="8">
         <v>3</v>
@@ -3013,7 +3010,7 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="20"/>
       <c r="Z23" s="19"/>
-      <c r="AA23" s="37">
+      <c r="AA23" s="28">
         <v>76.502815398853258</v>
       </c>
       <c r="AB23" s="8">
@@ -3025,7 +3022,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="21">
         <v>4</v>
@@ -3061,7 +3058,7 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="20"/>
       <c r="Z24" s="19"/>
-      <c r="AA24" s="37">
+      <c r="AA24" s="28">
         <v>0</v>
       </c>
       <c r="AB24" s="8">
@@ -3073,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3092,7 +3089,7 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="20"/>
       <c r="Z25" s="19"/>
-      <c r="AA25" s="37">
+      <c r="AA25" s="28">
         <v>10</v>
       </c>
       <c r="AB25" s="8">
@@ -3104,24 +3101,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="39">
-        <v>0</v>
-      </c>
-      <c r="D26" s="39">
+      <c r="C26" s="30">
+        <v>0</v>
+      </c>
+      <c r="D26" s="30">
         <v>1</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="30">
         <v>2</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="30">
         <v>3</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="30">
         <v>4</v>
       </c>
       <c r="H26" s="8"/>
@@ -3135,7 +3132,7 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="20"/>
       <c r="Z26" s="19"/>
-      <c r="AA26" s="37">
+      <c r="AA26" s="28">
         <v>20</v>
       </c>
       <c r="AB26" s="8">
@@ -3147,7 +3144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="21">
         <v>0</v>
@@ -3183,7 +3180,7 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="20"/>
       <c r="Z27" s="19"/>
-      <c r="AA27" s="37">
+      <c r="AA27" s="28">
         <v>20</v>
       </c>
       <c r="AB27" s="8">
@@ -3195,7 +3192,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="8">
         <v>1</v>
@@ -3230,20 +3227,20 @@
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="20"/>
-      <c r="Z28" s="46"/>
-      <c r="AA28" s="50">
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="38">
         <v>30</v>
       </c>
       <c r="AB28" s="10">
         <f t="shared" ref="AB28:AC28" si="16">F7</f>
         <v>0</v>
       </c>
-      <c r="AC28" s="47">
+      <c r="AC28" s="35">
         <f t="shared" si="16"/>
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="21">
         <v>2</v>
@@ -3279,20 +3276,20 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="20"/>
       <c r="Z29" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA29" s="49">
+        <v>36</v>
+      </c>
+      <c r="AA29" s="37">
         <f>T41</f>
         <v>-1000000</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC29" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="8">
         <v>3</v>
@@ -3333,13 +3330,13 @@
         <v>-999970</v>
       </c>
       <c r="AB30" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC30" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="21">
         <v>4</v>
@@ -3380,13 +3377,13 @@
         <v>-999960</v>
       </c>
       <c r="AB31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC31" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3410,30 +3407,30 @@
         <v>-999923.49718460126</v>
       </c>
       <c r="AB32" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC32" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="39">
-        <v>0</v>
-      </c>
-      <c r="D33" s="39">
+      <c r="C33" s="30">
+        <v>0</v>
+      </c>
+      <c r="D33" s="30">
         <v>1</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="30">
         <v>2</v>
       </c>
-      <c r="F33" s="39">
+      <c r="F33" s="30">
         <v>3</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="30">
         <v>4</v>
       </c>
       <c r="H33" s="8"/>
@@ -3452,13 +3449,13 @@
         <v>-999923.49718460115</v>
       </c>
       <c r="AB33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC33" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="21">
         <v>0</v>
@@ -3499,13 +3496,13 @@
         <v>-1000000</v>
       </c>
       <c r="AB34" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC34" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="8">
         <v>1</v>
@@ -3546,13 +3543,13 @@
         <v>-999990</v>
       </c>
       <c r="AB35" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC35" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="21">
         <v>2</v>
@@ -3584,24 +3581,24 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
-      <c r="O36" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="33"/>
+      <c r="O36" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="42"/>
       <c r="Z36" s="19"/>
       <c r="AA36" s="8">
         <f t="shared" si="22"/>
         <v>-999965.85786437627</v>
       </c>
       <c r="AB36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC36" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="8">
         <v>3</v>
@@ -3633,22 +3630,22 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="28"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="45"/>
       <c r="Z37" s="19"/>
       <c r="AA37" s="8">
         <f t="shared" si="22"/>
         <v>-999925.27864044998</v>
       </c>
       <c r="AB37" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC37" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="24">
         <v>4</v>
@@ -3680,97 +3677,97 @@
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
       <c r="N38" s="25"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="30"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="48"/>
       <c r="Z38" s="19"/>
       <c r="AA38" s="8">
         <f t="shared" si="22"/>
         <v>-999923.49718460115</v>
       </c>
       <c r="AB38" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC38" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Z39" s="19"/>
       <c r="AA39" s="7">
         <f>V41</f>
         <v>-10</v>
       </c>
       <c r="AB39" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC39" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="40">
-        <v>0</v>
-      </c>
-      <c r="D40" s="40">
+      <c r="C40" s="31">
+        <v>0</v>
+      </c>
+      <c r="D40" s="31">
         <v>1</v>
       </c>
-      <c r="E40" s="40">
+      <c r="E40" s="31">
         <v>2</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F40" s="31">
         <v>3</v>
       </c>
-      <c r="G40" s="40">
+      <c r="G40" s="31">
         <v>4</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="36" t="s">
+      <c r="I40" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J40" s="36" t="s">
+      <c r="J40" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K40" s="15"/>
-      <c r="L40" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40" s="40">
-        <v>0</v>
-      </c>
-      <c r="N40" s="40">
+      <c r="M40" s="31">
+        <v>0</v>
+      </c>
+      <c r="N40" s="31">
         <v>1</v>
       </c>
-      <c r="O40" s="40">
+      <c r="O40" s="31">
         <v>2</v>
       </c>
-      <c r="P40" s="40">
+      <c r="P40" s="31">
         <v>3</v>
       </c>
-      <c r="Q40" s="40">
+      <c r="Q40" s="31">
         <v>4</v>
       </c>
       <c r="R40" s="15"/>
-      <c r="S40" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="T40" s="40">
-        <v>0</v>
-      </c>
-      <c r="U40" s="40">
+      <c r="S40" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="T40" s="31">
+        <v>0</v>
+      </c>
+      <c r="U40" s="31">
         <v>1</v>
       </c>
-      <c r="V40" s="40">
+      <c r="V40" s="31">
         <v>2</v>
       </c>
-      <c r="W40" s="40">
+      <c r="W40" s="31">
         <v>3</v>
       </c>
-      <c r="X40" s="40">
+      <c r="X40" s="31">
         <v>4</v>
       </c>
       <c r="Y40" s="18"/>
@@ -3780,30 +3777,30 @@
         <v>-999985.85786437627</v>
       </c>
       <c r="AB40" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC40" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="21">
         <v>0</v>
       </c>
-      <c r="C41" s="37">
-        <v>0</v>
-      </c>
-      <c r="D41" s="37">
-        <v>0</v>
-      </c>
-      <c r="E41" s="37">
+      <c r="C41" s="28">
+        <v>0</v>
+      </c>
+      <c r="D41" s="28">
+        <v>0</v>
+      </c>
+      <c r="E41" s="28">
         <v>1</v>
       </c>
-      <c r="F41" s="37">
-        <v>0</v>
-      </c>
-      <c r="G41" s="37">
+      <c r="F41" s="28">
+        <v>0</v>
+      </c>
+      <c r="G41" s="28">
         <v>0</v>
       </c>
       <c r="H41" s="8"/>
@@ -3844,23 +3841,23 @@
         <v>0</v>
       </c>
       <c r="T41" s="8">
-        <f>$AA19+C34+$H3-T$55-$K$2*(1-C41)</f>
+        <f t="shared" ref="T41:X45" si="28">$AA19+C34+$H3-T$55-$K$2*(1-C41)</f>
         <v>-1000000</v>
       </c>
       <c r="U41" s="8">
-        <f>$AA19+D34+$H3-U$55-$K$2*(1-D41)</f>
+        <f t="shared" si="28"/>
         <v>-1000000</v>
       </c>
       <c r="V41" s="8">
-        <f>$AA19+E34+$H3-V$55-$K$2*(1-E41)</f>
+        <f t="shared" si="28"/>
         <v>-10</v>
       </c>
       <c r="W41" s="8">
-        <f>$AA19+F34+$H3-W$55-$K$2*(1-F41)</f>
+        <f t="shared" si="28"/>
         <v>-1000038.2185441513</v>
       </c>
       <c r="X41" s="8">
-        <f>$AA19+G34+$H3-X$55-$K$2*(1-G41)</f>
+        <f t="shared" si="28"/>
         <v>-1000076.5028153989</v>
       </c>
       <c r="Y41" s="20"/>
@@ -3870,39 +3867,39 @@
         <v>-999990</v>
       </c>
       <c r="AB41" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC41" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="8">
         <v>1</v>
       </c>
-      <c r="C42" s="37">
-        <v>0</v>
-      </c>
-      <c r="D42" s="37">
-        <v>0</v>
-      </c>
-      <c r="E42" s="37">
-        <v>0</v>
-      </c>
-      <c r="F42" s="37">
-        <v>0</v>
-      </c>
-      <c r="G42" s="37">
+      <c r="C42" s="28">
+        <v>0</v>
+      </c>
+      <c r="D42" s="28">
+        <v>0</v>
+      </c>
+      <c r="E42" s="28">
+        <v>0</v>
+      </c>
+      <c r="F42" s="28">
+        <v>0</v>
+      </c>
+      <c r="G42" s="28">
         <v>0</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="8">
-        <f t="shared" ref="I42:I45" si="28">E4</f>
+        <f t="shared" ref="I42:I45" si="29">E4</f>
         <v>10</v>
       </c>
       <c r="J42" s="8">
-        <f t="shared" ref="J42:J45" si="29">SUM(C42:G42)*I42</f>
+        <f t="shared" ref="J42:J45" si="30">SUM(C42:G42)*I42</f>
         <v>0</v>
       </c>
       <c r="K42" s="8"/>
@@ -3910,23 +3907,23 @@
         <v>1</v>
       </c>
       <c r="M42" s="8">
-        <f t="shared" ref="M42:M45" si="30">C42*C28</f>
+        <f t="shared" ref="M42:M45" si="31">C42*C28</f>
         <v>0</v>
       </c>
       <c r="N42" s="8">
-        <f t="shared" ref="N42:N45" si="31">D42*D28</f>
+        <f t="shared" ref="N42:N45" si="32">D42*D28</f>
         <v>0</v>
       </c>
       <c r="O42" s="8">
-        <f t="shared" ref="O42:O45" si="32">E42*E28</f>
+        <f t="shared" ref="O42:O45" si="33">E42*E28</f>
         <v>0</v>
       </c>
       <c r="P42" s="8">
-        <f t="shared" ref="P42:P45" si="33">F42*F28</f>
+        <f t="shared" ref="P42:P45" si="34">F42*F28</f>
         <v>0</v>
       </c>
       <c r="Q42" s="8">
-        <f t="shared" ref="Q42:Q45" si="34">G42*G28</f>
+        <f t="shared" ref="Q42:Q45" si="35">G42*G28</f>
         <v>0</v>
       </c>
       <c r="R42" s="8"/>
@@ -3934,23 +3931,23 @@
         <v>1</v>
       </c>
       <c r="T42" s="8">
-        <f>$AA20+C35+$H4-T$55-$K$2*(1-C42)</f>
+        <f t="shared" si="28"/>
         <v>-999970</v>
       </c>
       <c r="U42" s="8">
-        <f>$AA20+D35+$H4-U$55-$K$2*(1-D42)</f>
+        <f t="shared" si="28"/>
         <v>-999990</v>
       </c>
       <c r="V42" s="8">
-        <f>$AA20+E35+$H4-V$55-$K$2*(1-E42)</f>
+        <f t="shared" si="28"/>
         <v>-999985.85786437627</v>
       </c>
       <c r="W42" s="8">
-        <f>$AA20+F35+$H4-W$55-$K$2*(1-F42)</f>
+        <f t="shared" si="28"/>
         <v>-1000010</v>
       </c>
       <c r="X42" s="8">
-        <f>$AA20+G35+$H4-X$55-$K$2*(1-G42)</f>
+        <f t="shared" si="28"/>
         <v>-1000046.5028153989</v>
       </c>
       <c r="Y42" s="20"/>
@@ -3960,39 +3957,39 @@
         <v>-999935.27864044998</v>
       </c>
       <c r="AB42" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC42" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="21">
         <v>2</v>
       </c>
-      <c r="C43" s="37">
-        <v>0</v>
-      </c>
-      <c r="D43" s="37">
-        <v>0</v>
-      </c>
-      <c r="E43" s="37">
-        <v>0</v>
-      </c>
-      <c r="F43" s="37">
+      <c r="C43" s="28">
+        <v>0</v>
+      </c>
+      <c r="D43" s="28">
+        <v>0</v>
+      </c>
+      <c r="E43" s="28">
+        <v>0</v>
+      </c>
+      <c r="F43" s="28">
         <v>1</v>
       </c>
-      <c r="G43" s="37">
+      <c r="G43" s="28">
         <v>0</v>
       </c>
       <c r="H43" s="8"/>
       <c r="I43" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7</v>
       </c>
       <c r="J43" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="K43" s="8"/>
@@ -4000,23 +3997,23 @@
         <v>2</v>
       </c>
       <c r="M43" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N43" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O43" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P43" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>22.360679774997898</v>
       </c>
       <c r="Q43" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="R43" s="8"/>
@@ -4024,23 +4021,23 @@
         <v>2</v>
       </c>
       <c r="T43" s="8">
-        <f>$AA21+C36+$H5-T$55-$K$2*(1-C43)</f>
+        <f t="shared" si="28"/>
         <v>-999960</v>
       </c>
       <c r="U43" s="8">
-        <f>$AA21+D36+$H5-U$55-$K$2*(1-D43)</f>
+        <f t="shared" si="28"/>
         <v>-999965.85786437627</v>
       </c>
       <c r="V43" s="8">
-        <f>$AA21+E36+$H5-V$55-$K$2*(1-E43)</f>
+        <f t="shared" si="28"/>
         <v>-999990</v>
       </c>
       <c r="W43" s="8">
-        <f>$AA21+F36+$H5-W$55-$K$2*(1-F43)</f>
+        <f t="shared" si="28"/>
         <v>-1.2882139799330616E-11</v>
       </c>
       <c r="X43" s="8">
-        <f>$AA21+G36+$H5-X$55-$K$2*(1-G43)</f>
+        <f t="shared" si="28"/>
         <v>-1000036.5028153989</v>
       </c>
       <c r="Y43" s="20"/>
@@ -4050,39 +4047,39 @@
         <v>-999933.49718460115</v>
       </c>
       <c r="AB43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC43" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="8">
         <v>3</v>
       </c>
-      <c r="C44" s="37">
-        <v>0</v>
-      </c>
-      <c r="D44" s="37">
-        <v>0</v>
-      </c>
-      <c r="E44" s="37">
-        <v>0</v>
-      </c>
-      <c r="F44" s="37">
-        <v>0</v>
-      </c>
-      <c r="G44" s="37">
+      <c r="C44" s="28">
+        <v>0</v>
+      </c>
+      <c r="D44" s="28">
+        <v>0</v>
+      </c>
+      <c r="E44" s="28">
+        <v>0</v>
+      </c>
+      <c r="F44" s="28">
+        <v>0</v>
+      </c>
+      <c r="G44" s="28">
         <v>1</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>13</v>
       </c>
       <c r="J44" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>13</v>
       </c>
       <c r="K44" s="8"/>
@@ -4090,23 +4087,23 @@
         <v>3</v>
       </c>
       <c r="M44" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N44" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O44" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="Q44" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>14.142135623730951</v>
       </c>
       <c r="R44" s="8"/>
@@ -4114,23 +4111,23 @@
         <v>3</v>
       </c>
       <c r="T44" s="8">
-        <f>$AA22+C37+$H6-T$55-$K$2*(1-C44)</f>
+        <f t="shared" si="28"/>
         <v>-999923.49718460126</v>
       </c>
       <c r="U44" s="8">
-        <f>$AA22+D37+$H6-U$55-$K$2*(1-D44)</f>
+        <f t="shared" si="28"/>
         <v>-999925.27864044998</v>
       </c>
       <c r="V44" s="8">
-        <f>$AA22+E37+$H6-V$55-$K$2*(1-E44)</f>
+        <f t="shared" si="28"/>
         <v>-999935.27864044998</v>
       </c>
       <c r="W44" s="8">
-        <f>$AA22+F37+$H6-W$55-$K$2*(1-F44)</f>
+        <f t="shared" si="28"/>
         <v>-999990</v>
       </c>
       <c r="X44" s="8">
-        <f>$AA22+G37+$H6-X$55-$K$2*(1-G44)</f>
+        <f t="shared" si="28"/>
         <v>-1.1152678780490533E-10</v>
       </c>
       <c r="Y44" s="20"/>
@@ -4140,39 +4137,39 @@
         <v>-1000038.2185441513</v>
       </c>
       <c r="AB44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC44" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="21">
         <v>4</v>
       </c>
-      <c r="C45" s="37">
-        <v>0</v>
-      </c>
-      <c r="D45" s="37">
-        <v>0</v>
-      </c>
-      <c r="E45" s="37">
-        <v>0</v>
-      </c>
-      <c r="F45" s="37">
-        <v>0</v>
-      </c>
-      <c r="G45" s="37">
+      <c r="C45" s="28">
+        <v>0</v>
+      </c>
+      <c r="D45" s="28">
+        <v>0</v>
+      </c>
+      <c r="E45" s="28">
+        <v>0</v>
+      </c>
+      <c r="F45" s="28">
+        <v>0</v>
+      </c>
+      <c r="G45" s="28">
         <v>0</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="K45" s="8"/>
@@ -4180,23 +4177,23 @@
         <v>4</v>
       </c>
       <c r="M45" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N45" s="8">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O45" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P45" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="Q45" s="8">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="R45" s="8"/>
@@ -4204,39 +4201,39 @@
         <v>4</v>
       </c>
       <c r="T45" s="8">
-        <f>$AA23+C38+$H7-T$55-$K$2*(1-C45)</f>
+        <f t="shared" si="28"/>
         <v>-999923.49718460115</v>
       </c>
       <c r="U45" s="8">
-        <f>$AA23+D38+$H7-U$55-$K$2*(1-D45)</f>
+        <f t="shared" si="28"/>
         <v>-999923.49718460115</v>
       </c>
       <c r="V45" s="8">
-        <f>$AA23+E38+$H7-V$55-$K$2*(1-E45)</f>
+        <f t="shared" si="28"/>
         <v>-999933.49718460115</v>
       </c>
       <c r="W45" s="8">
-        <f>$AA23+F38+$H7-W$55-$K$2*(1-F45)</f>
+        <f t="shared" si="28"/>
         <v>-999961.71572875243</v>
       </c>
       <c r="X45" s="8">
-        <f>$AA23+G38+$H7-X$55-$K$2*(1-G45)</f>
+        <f t="shared" si="28"/>
         <v>-1000000</v>
       </c>
       <c r="Y45" s="20"/>
       <c r="Z45" s="8"/>
       <c r="AA45" s="8">
-        <f t="shared" ref="AA45:AA47" si="35">W42</f>
+        <f t="shared" ref="AA45:AA47" si="36">W42</f>
         <v>-1000010</v>
       </c>
       <c r="AB45" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC45" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -4264,34 +4261,34 @@
       <c r="Y46" s="20"/>
       <c r="Z46" s="8"/>
       <c r="AA46" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-1.2882139799330616E-11</v>
       </c>
       <c r="AB46" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC46" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="39">
-        <v>0</v>
-      </c>
-      <c r="D47" s="39">
+        <v>25</v>
+      </c>
+      <c r="C47" s="30">
+        <v>0</v>
+      </c>
+      <c r="D47" s="30">
         <v>1</v>
       </c>
-      <c r="E47" s="39">
+      <c r="E47" s="30">
         <v>2</v>
       </c>
-      <c r="F47" s="39">
+      <c r="F47" s="30">
         <v>3</v>
       </c>
-      <c r="G47" s="39">
+      <c r="G47" s="30">
         <v>4</v>
       </c>
       <c r="H47" s="8"/>
@@ -4299,77 +4296,77 @@
         <v>19</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M47" s="39">
-        <v>0</v>
-      </c>
-      <c r="N47" s="39">
+        <v>20</v>
+      </c>
+      <c r="M47" s="30">
+        <v>0</v>
+      </c>
+      <c r="N47" s="30">
         <v>1</v>
       </c>
-      <c r="O47" s="39">
+      <c r="O47" s="30">
         <v>2</v>
       </c>
-      <c r="P47" s="39">
+      <c r="P47" s="30">
         <v>3</v>
       </c>
-      <c r="Q47" s="39">
+      <c r="Q47" s="30">
         <v>4</v>
       </c>
       <c r="R47" s="8"/>
       <c r="S47" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="T47" s="39">
-        <v>0</v>
-      </c>
-      <c r="U47" s="39">
+        <v>24</v>
+      </c>
+      <c r="T47" s="30">
+        <v>0</v>
+      </c>
+      <c r="U47" s="30">
         <v>1</v>
       </c>
-      <c r="V47" s="39">
+      <c r="V47" s="30">
         <v>2</v>
       </c>
-      <c r="W47" s="39">
+      <c r="W47" s="30">
         <v>3</v>
       </c>
-      <c r="X47" s="39">
+      <c r="X47" s="30">
         <v>4</v>
       </c>
       <c r="Y47" s="20"/>
       <c r="Z47" s="8"/>
       <c r="AA47" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-999990</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC47" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="21">
         <v>0</v>
       </c>
-      <c r="C48" s="37">
-        <v>0</v>
-      </c>
-      <c r="D48" s="37">
+      <c r="C48" s="28">
+        <v>0</v>
+      </c>
+      <c r="D48" s="28">
         <v>1</v>
       </c>
-      <c r="E48" s="37">
-        <v>0</v>
-      </c>
-      <c r="F48" s="37">
-        <v>0</v>
-      </c>
-      <c r="G48" s="37">
+      <c r="E48" s="28">
+        <v>0</v>
+      </c>
+      <c r="F48" s="28">
+        <v>0</v>
+      </c>
+      <c r="G48" s="28">
         <v>0</v>
       </c>
       <c r="H48" s="8"/>
@@ -4390,19 +4387,19 @@
         <v>0</v>
       </c>
       <c r="N48" s="8">
-        <f t="shared" ref="N48:Q48" si="36">D48*D27</f>
+        <f t="shared" ref="N48:Q48" si="37">D48*D27</f>
         <v>10</v>
       </c>
       <c r="O48" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P48" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Q48" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="R48" s="8"/>
@@ -4410,23 +4407,23 @@
         <v>0</v>
       </c>
       <c r="T48" s="8">
-        <f>$AA24+C34+$H3-T$56-$K$2*(1-C48)</f>
+        <f t="shared" ref="T48:X52" si="38">$AA24+C34+$H3-T$56-$K$2*(1-C48)</f>
         <v>-1000000</v>
       </c>
       <c r="U48" s="8">
-        <f>$AA24+D34+$H3-U$56-$K$2*(1-D48)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V48" s="8">
-        <f>$AA24+E34+$H3-V$56-$K$2*(1-E48)</f>
+        <f t="shared" si="38"/>
         <v>-1000010</v>
       </c>
       <c r="W48" s="8">
-        <f>$AA24+F34+$H3-W$56-$K$2*(1-F48)</f>
+        <f t="shared" si="38"/>
         <v>-1000005.8578643763</v>
       </c>
       <c r="X48" s="8">
-        <f>$AA24+G34+$H3-X$56-$K$2*(1-G48)</f>
+        <f t="shared" si="38"/>
         <v>-1000030</v>
       </c>
       <c r="Y48" s="20"/>
@@ -4436,39 +4433,39 @@
         <v>-999961.71572875243</v>
       </c>
       <c r="AB48" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC48" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="8">
         <v>1</v>
       </c>
-      <c r="C49" s="37">
-        <v>0</v>
-      </c>
-      <c r="D49" s="37">
-        <v>0</v>
-      </c>
-      <c r="E49" s="37">
-        <v>0</v>
-      </c>
-      <c r="F49" s="37">
-        <v>0</v>
-      </c>
-      <c r="G49" s="37">
+      <c r="C49" s="28">
+        <v>0</v>
+      </c>
+      <c r="D49" s="28">
+        <v>0</v>
+      </c>
+      <c r="E49" s="28">
+        <v>0</v>
+      </c>
+      <c r="F49" s="28">
+        <v>0</v>
+      </c>
+      <c r="G49" s="28">
         <v>1</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8">
-        <f t="shared" ref="I49:I52" si="37">E4</f>
+        <f t="shared" ref="I49:I52" si="39">E4</f>
         <v>10</v>
       </c>
       <c r="J49" s="8">
-        <f t="shared" ref="J49:J52" si="38">SUM(C49:G49)*I49</f>
+        <f t="shared" ref="J49:J52" si="40">SUM(C49:G49)*I49</f>
         <v>10</v>
       </c>
       <c r="K49" s="8"/>
@@ -4476,23 +4473,23 @@
         <v>1</v>
       </c>
       <c r="M49" s="8">
-        <f t="shared" ref="M49:M52" si="39">C49*C28</f>
+        <f t="shared" ref="M49:M52" si="41">C49*C28</f>
         <v>0</v>
       </c>
       <c r="N49" s="8">
-        <f t="shared" ref="N49:N52" si="40">D49*D28</f>
+        <f t="shared" ref="N49:N52" si="42">D49*D28</f>
         <v>0</v>
       </c>
       <c r="O49" s="8">
-        <f t="shared" ref="O49:O52" si="41">E49*E28</f>
+        <f t="shared" ref="O49:O52" si="43">E49*E28</f>
         <v>0</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" ref="P49:P52" si="42">F49*F28</f>
+        <f t="shared" ref="P49:P52" si="44">F49*F28</f>
         <v>0</v>
       </c>
       <c r="Q49" s="8">
-        <f t="shared" ref="Q49:Q52" si="43">G49*G28</f>
+        <f t="shared" ref="Q49:Q52" si="45">G49*G28</f>
         <v>10</v>
       </c>
       <c r="R49" s="8"/>
@@ -4500,23 +4497,23 @@
         <v>1</v>
       </c>
       <c r="T49" s="8">
-        <f>$AA25+C35+$H4-T$56-$K$2*(1-C49)</f>
+        <f t="shared" si="38"/>
         <v>-999970</v>
       </c>
       <c r="U49" s="8">
-        <f>$AA25+D35+$H4-U$56-$K$2*(1-D49)</f>
+        <f t="shared" si="38"/>
         <v>-999990</v>
       </c>
       <c r="V49" s="8">
-        <f>$AA25+E35+$H4-V$56-$K$2*(1-E49)</f>
+        <f t="shared" si="38"/>
         <v>-999985.85786437627</v>
       </c>
       <c r="W49" s="8">
-        <f>$AA25+F35+$H4-W$56-$K$2*(1-F49)</f>
+        <f t="shared" si="38"/>
         <v>-999977.63932022499</v>
       </c>
       <c r="X49" s="8">
-        <f>$AA25+G35+$H4-X$56-$K$2*(1-G49)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y49" s="20"/>
@@ -4526,39 +4523,39 @@
         <v>-1000076.5028153989</v>
       </c>
       <c r="AB49" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC49" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="21">
         <v>2</v>
       </c>
-      <c r="C50" s="37">
-        <v>0</v>
-      </c>
-      <c r="D50" s="37">
-        <v>0</v>
-      </c>
-      <c r="E50" s="37">
-        <v>0</v>
-      </c>
-      <c r="F50" s="37">
-        <v>0</v>
-      </c>
-      <c r="G50" s="37">
+      <c r="C50" s="28">
+        <v>0</v>
+      </c>
+      <c r="D50" s="28">
+        <v>0</v>
+      </c>
+      <c r="E50" s="28">
+        <v>0</v>
+      </c>
+      <c r="F50" s="28">
+        <v>0</v>
+      </c>
+      <c r="G50" s="28">
         <v>0</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
       <c r="J50" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K50" s="8"/>
@@ -4566,23 +4563,23 @@
         <v>2</v>
       </c>
       <c r="M50" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N50" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O50" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="P50" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Q50" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="R50" s="8"/>
@@ -4590,65 +4587,65 @@
         <v>2</v>
       </c>
       <c r="T50" s="8">
-        <f>$AA26+C36+$H5-T$56-$K$2*(1-C50)</f>
+        <f t="shared" si="38"/>
         <v>-999960</v>
       </c>
       <c r="U50" s="8">
-        <f>$AA26+D36+$H5-U$56-$K$2*(1-D50)</f>
+        <f t="shared" si="38"/>
         <v>-999965.85786437627</v>
       </c>
       <c r="V50" s="8">
-        <f>$AA26+E36+$H5-V$56-$K$2*(1-E50)</f>
+        <f t="shared" si="38"/>
         <v>-999990</v>
       </c>
       <c r="W50" s="8">
-        <f>$AA26+F36+$H5-W$56-$K$2*(1-F50)</f>
+        <f t="shared" si="38"/>
         <v>-999967.63932022499</v>
       </c>
       <c r="X50" s="8">
-        <f>$AA26+G36+$H5-X$56-$K$2*(1-G50)</f>
+        <f t="shared" si="38"/>
         <v>-999990</v>
       </c>
       <c r="Y50" s="20"/>
       <c r="Z50" s="8"/>
       <c r="AA50" s="7">
-        <f t="shared" ref="AA50:AA53" si="44">X42</f>
+        <f t="shared" ref="AA50:AA53" si="46">X42</f>
         <v>-1000046.5028153989</v>
       </c>
       <c r="AB50" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC50" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="8">
         <v>3</v>
       </c>
-      <c r="C51" s="37">
-        <v>0</v>
-      </c>
-      <c r="D51" s="37">
-        <v>0</v>
-      </c>
-      <c r="E51" s="37">
-        <v>0</v>
-      </c>
-      <c r="F51" s="37">
-        <v>0</v>
-      </c>
-      <c r="G51" s="37">
+      <c r="C51" s="28">
+        <v>0</v>
+      </c>
+      <c r="D51" s="28">
+        <v>0</v>
+      </c>
+      <c r="E51" s="28">
+        <v>0</v>
+      </c>
+      <c r="F51" s="28">
+        <v>0</v>
+      </c>
+      <c r="G51" s="28">
         <v>0</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>13</v>
       </c>
       <c r="J51" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K51" s="8"/>
@@ -4656,23 +4653,23 @@
         <v>3</v>
       </c>
       <c r="M51" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N51" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O51" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="P51" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Q51" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="R51" s="8"/>
@@ -4680,65 +4677,65 @@
         <v>3</v>
       </c>
       <c r="T51" s="8">
-        <f>$AA27+C37+$H6-T$56-$K$2*(1-C51)</f>
+        <f t="shared" si="38"/>
         <v>-999955.85786437627</v>
       </c>
       <c r="U51" s="8">
-        <f>$AA27+D37+$H6-U$56-$K$2*(1-D51)</f>
+        <f t="shared" si="38"/>
         <v>-999957.63932022499</v>
       </c>
       <c r="V51" s="8">
-        <f>$AA27+E37+$H6-V$56-$K$2*(1-E51)</f>
+        <f t="shared" si="38"/>
         <v>-999967.63932022499</v>
       </c>
       <c r="W51" s="8">
-        <f>$AA27+F37+$H6-W$56-$K$2*(1-F51)</f>
+        <f t="shared" si="38"/>
         <v>-999990</v>
       </c>
       <c r="X51" s="8">
-        <f>$AA27+G37+$H6-X$56-$K$2*(1-G51)</f>
+        <f t="shared" si="38"/>
         <v>-999985.85786437627</v>
       </c>
       <c r="Y51" s="20"/>
       <c r="Z51" s="8"/>
       <c r="AA51" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>-1000036.5028153989</v>
       </c>
       <c r="AB51" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC51" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="19"/>
       <c r="B52" s="21">
         <v>4</v>
       </c>
-      <c r="C52" s="37">
-        <v>0</v>
-      </c>
-      <c r="D52" s="37">
-        <v>0</v>
-      </c>
-      <c r="E52" s="37">
-        <v>0</v>
-      </c>
-      <c r="F52" s="37">
-        <v>0</v>
-      </c>
-      <c r="G52" s="37">
+      <c r="C52" s="28">
+        <v>0</v>
+      </c>
+      <c r="D52" s="28">
+        <v>0</v>
+      </c>
+      <c r="E52" s="28">
+        <v>0</v>
+      </c>
+      <c r="F52" s="28">
+        <v>0</v>
+      </c>
+      <c r="G52" s="28">
         <v>0</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K52" s="8"/>
@@ -4746,23 +4743,23 @@
         <v>4</v>
       </c>
       <c r="M52" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N52" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O52" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="P52" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Q52" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="R52" s="8"/>
@@ -4770,39 +4767,39 @@
         <v>4</v>
       </c>
       <c r="T52" s="8">
-        <f>$AA28+C38+$H7-T$56-$K$2*(1-C52)</f>
+        <f t="shared" si="38"/>
         <v>-999970</v>
       </c>
       <c r="U52" s="8">
-        <f>$AA28+D38+$H7-U$56-$K$2*(1-D52)</f>
+        <f t="shared" si="38"/>
         <v>-999970</v>
       </c>
       <c r="V52" s="8">
-        <f>$AA28+E38+$H7-V$56-$K$2*(1-E52)</f>
+        <f t="shared" si="38"/>
         <v>-999980</v>
       </c>
       <c r="W52" s="8">
-        <f>$AA28+F38+$H7-W$56-$K$2*(1-F52)</f>
+        <f t="shared" si="38"/>
         <v>-999975.85786437627</v>
       </c>
       <c r="X52" s="8">
-        <f>$AA28+G38+$H7-X$56-$K$2*(1-G52)</f>
+        <f t="shared" si="38"/>
         <v>-1000000</v>
       </c>
       <c r="Y52" s="20"/>
       <c r="Z52" s="8"/>
       <c r="AA52" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>-1.1152678780490533E-10</v>
       </c>
       <c r="AB52" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC52" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="19"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -4828,27 +4825,27 @@
       <c r="W53" s="8"/>
       <c r="X53" s="8"/>
       <c r="Y53" s="20"/>
-      <c r="Z53" s="46"/>
-      <c r="AA53" s="51">
-        <f t="shared" si="44"/>
+      <c r="Z53" s="34"/>
+      <c r="AA53" s="39">
+        <f t="shared" si="46"/>
         <v>-1000000</v>
       </c>
       <c r="AB53" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC53" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="AC53" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="19"/>
       <c r="B54" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
@@ -4858,21 +4855,21 @@
       <c r="K54" s="8"/>
       <c r="R54" s="8"/>
       <c r="S54" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="T54" s="39">
-        <v>0</v>
-      </c>
-      <c r="U54" s="39">
+        <v>21</v>
+      </c>
+      <c r="T54" s="30">
+        <v>0</v>
+      </c>
+      <c r="U54" s="30">
         <v>1</v>
       </c>
-      <c r="V54" s="39">
+      <c r="V54" s="30">
         <v>2</v>
       </c>
-      <c r="W54" s="39">
+      <c r="W54" s="30">
         <v>3</v>
       </c>
-      <c r="X54" s="39">
+      <c r="X54" s="30">
         <v>4</v>
       </c>
       <c r="Y54" s="20"/>
@@ -4882,13 +4879,13 @@
         <v>-1000000</v>
       </c>
       <c r="AB54" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC54" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="19"/>
       <c r="B55" s="21">
         <v>0</v>
@@ -4911,43 +4908,43 @@
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
       <c r="R55" s="8"/>
-      <c r="S55" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="T55" s="37">
+      <c r="S55" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="T55" s="28">
         <f>AA19</f>
         <v>0</v>
       </c>
-      <c r="U55" s="37">
+      <c r="U55" s="28">
         <f>AA20</f>
         <v>10</v>
       </c>
-      <c r="V55" s="37">
+      <c r="V55" s="28">
         <f>AA21</f>
         <v>20</v>
       </c>
-      <c r="W55" s="37">
+      <c r="W55" s="28">
         <f>AA22</f>
         <v>52.36067977501078</v>
       </c>
-      <c r="X55" s="37">
+      <c r="X55" s="28">
         <f>AA23</f>
         <v>76.502815398853258</v>
       </c>
       <c r="Y55" s="20"/>
       <c r="Z55" s="8"/>
       <c r="AA55" s="8">
-        <f t="shared" ref="AA55:AA58" si="45">T49</f>
+        <f t="shared" ref="AA55:AA58" si="47">T49</f>
         <v>-999970</v>
       </c>
       <c r="AB55" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC55" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="19"/>
       <c r="B56" s="8">
         <v>1</v>
@@ -4961,7 +4958,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="8">
-        <f t="shared" ref="F56:F59" si="46">_xlfn.XMATCH(1,C49:G49)-1</f>
+        <f t="shared" ref="F56:F59" si="48">_xlfn.XMATCH(1,C49:G49)-1</f>
         <v>4</v>
       </c>
       <c r="G56" s="8"/>
@@ -4970,49 +4967,49 @@
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="R56" s="8"/>
-      <c r="S56" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="T56" s="37">
+      <c r="S56" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="T56" s="28">
         <f>AA24</f>
         <v>0</v>
       </c>
-      <c r="U56" s="37">
+      <c r="U56" s="28">
         <f>AA25</f>
         <v>10</v>
       </c>
-      <c r="V56" s="37">
+      <c r="V56" s="28">
         <f>AA26</f>
         <v>20</v>
       </c>
-      <c r="W56" s="37">
+      <c r="W56" s="28">
         <f>AA27</f>
         <v>20</v>
       </c>
-      <c r="X56" s="37">
+      <c r="X56" s="28">
         <f>AA28</f>
         <v>30</v>
       </c>
       <c r="Y56" s="20"/>
       <c r="Z56" s="8"/>
       <c r="AA56" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-999960</v>
       </c>
       <c r="AB56" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC56" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="21">
         <v>2</v>
       </c>
       <c r="C57" s="8">
-        <f t="shared" ref="C57:C59" si="47">_xlfn.XMATCH(1,C43:G43)-1</f>
+        <f t="shared" ref="C57:C59" si="49">_xlfn.XMATCH(1,C43:G43)-1</f>
         <v>3</v>
       </c>
       <c r="D57" s="8"/>
@@ -5020,7 +5017,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="8" t="e">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>#N/A</v>
       </c>
       <c r="G57" s="8"/>
@@ -5039,28 +5036,28 @@
       <c r="T57" s="8"/>
       <c r="U57" s="8"/>
       <c r="V57" s="8"/>
-      <c r="W57" s="44"/>
-      <c r="X57" s="44"/>
-      <c r="Y57" s="45"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="32"/>
+      <c r="Y57" s="33"/>
       <c r="Z57" s="8"/>
       <c r="AA57" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-999955.85786437627</v>
       </c>
       <c r="AB57" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC57" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="19"/>
       <c r="B58" s="8">
         <v>3</v>
       </c>
       <c r="C58" s="8">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>4</v>
       </c>
       <c r="D58" s="8"/>
@@ -5068,7 +5065,7 @@
         <v>3</v>
       </c>
       <c r="F58" s="8" t="e">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>#N/A</v>
       </c>
       <c r="G58" s="8"/>
@@ -5087,30 +5084,30 @@
       <c r="T58" s="8"/>
       <c r="U58" s="8"/>
       <c r="V58" s="8"/>
-      <c r="W58" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="X58" s="32"/>
-      <c r="Y58" s="33"/>
+      <c r="W58" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="X58" s="41"/>
+      <c r="Y58" s="42"/>
       <c r="Z58" s="8"/>
       <c r="AA58" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>-999970</v>
       </c>
       <c r="AB58" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC58" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="24">
         <v>4</v>
       </c>
       <c r="C59" s="25" t="e">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>#N/A</v>
       </c>
       <c r="D59" s="25"/>
@@ -5118,7 +5115,7 @@
         <v>4</v>
       </c>
       <c r="F59" s="25" t="e">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>#N/A</v>
       </c>
       <c r="G59" s="25"/>
@@ -5137,265 +5134,265 @@
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
       <c r="V59" s="25"/>
-      <c r="W59" s="35"/>
-      <c r="X59" s="29"/>
-      <c r="Y59" s="30"/>
+      <c r="W59" s="46"/>
+      <c r="X59" s="47"/>
+      <c r="Y59" s="48"/>
       <c r="Z59" s="8"/>
       <c r="AA59" s="7">
         <f>U48</f>
         <v>0</v>
       </c>
       <c r="AB59" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC59" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Z60" s="19"/>
       <c r="AA60" s="7">
         <f>U49</f>
         <v>-999990</v>
       </c>
       <c r="AB60" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC60" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Z61" s="19"/>
       <c r="AA61" s="7">
         <f>U50</f>
         <v>-999965.85786437627</v>
       </c>
       <c r="AB61" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC61" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Z62" s="19"/>
       <c r="AA62" s="7">
         <f>U51</f>
         <v>-999957.63932022499</v>
       </c>
       <c r="AB62" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC62" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Z63" s="19"/>
       <c r="AA63" s="7">
         <f>U52</f>
         <v>-999970</v>
       </c>
       <c r="AB63" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC63" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Z64" s="19"/>
       <c r="AA64" s="8">
         <f>V48</f>
         <v>-1000010</v>
       </c>
       <c r="AB64" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC64" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="65" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z65" s="19"/>
       <c r="AA65" s="8">
         <f>V49</f>
         <v>-999985.85786437627</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC65" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="66" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z66" s="19"/>
       <c r="AA66" s="8">
         <f>V50</f>
         <v>-999990</v>
       </c>
       <c r="AB66" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC66" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="67" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z67" s="19"/>
       <c r="AA67" s="8">
         <f>V51</f>
         <v>-999967.63932022499</v>
       </c>
       <c r="AB67" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC67" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="68" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z68" s="19"/>
       <c r="AA68" s="8">
         <f>V52</f>
         <v>-999980</v>
       </c>
       <c r="AB68" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC68" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="69" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z69" s="19"/>
       <c r="AA69" s="7">
         <f>W48</f>
         <v>-1000005.8578643763</v>
       </c>
       <c r="AB69" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC69" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="70" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z70" s="19"/>
       <c r="AA70" s="7">
         <f>W49</f>
         <v>-999977.63932022499</v>
       </c>
       <c r="AB70" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC70" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="71" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z71" s="19"/>
       <c r="AA71" s="7">
         <f>W50</f>
         <v>-999967.63932022499</v>
       </c>
       <c r="AB71" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC71" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="72" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z72" s="19"/>
       <c r="AA72" s="7">
         <f>W51</f>
         <v>-999990</v>
       </c>
       <c r="AB72" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC72" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="73" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z73" s="19"/>
       <c r="AA73" s="7">
         <f>W52</f>
         <v>-999975.85786437627</v>
       </c>
       <c r="AB73" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC73" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="26:29" x14ac:dyDescent="0.35">
+    <row r="74" spans="26:29" x14ac:dyDescent="0.2">
       <c r="Z74" s="19"/>
       <c r="AA74" s="8">
         <f>X48</f>
         <v>-1000030</v>
       </c>
       <c r="AB74" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC74" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="26:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="26:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Z75" s="19"/>
       <c r="AA75" s="8">
         <f>X49</f>
         <v>0</v>
       </c>
       <c r="AB75" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC75" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="26:29" x14ac:dyDescent="0.35">
-      <c r="Z76" s="41" t="s">
-        <v>42</v>
+    <row r="76" spans="26:29" x14ac:dyDescent="0.2">
+      <c r="Z76" s="49" t="s">
+        <v>41</v>
       </c>
       <c r="AA76" s="8">
         <f>X50</f>
         <v>-999990</v>
       </c>
       <c r="AB76" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC76" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="26:29" x14ac:dyDescent="0.35">
-      <c r="Z77" s="42"/>
+    <row r="77" spans="26:29" x14ac:dyDescent="0.2">
+      <c r="Z77" s="50"/>
       <c r="AA77" s="8">
         <f>X51</f>
         <v>-999985.85786437627</v>
       </c>
       <c r="AB77" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC77" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="26:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="Z78" s="43"/>
+    <row r="78" spans="26:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Z78" s="51"/>
       <c r="AA78" s="25">
         <f>X52</f>
         <v>-1000000</v>
       </c>
       <c r="AB78" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC78" s="26">
         <v>0</v>

</xml_diff>